<commit_message>
Fields with yes and OK
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -95,7 +95,7 @@
     <t>13. Create  a community using the Napili Template</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>Yes_OK</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>